<commit_message>
update angle and acceleration detection
</commit_message>
<xml_diff>
--- a/displacement unidirection/steps mpu.xlsx
+++ b/displacement unidirection/steps mpu.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b421ec9807905863/Documents/Wireless SDP/Wireless-SDP/displacement unidirection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conce\OneDrive\Documents\Wireless SDP\Wireless-SDP\displacement unidirection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{8A0D9DC5-5C72-4622-8027-B5A83E0C1612}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{22143DE0-BEBF-4C23-9C3A-5314985F2F68}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{8A0D9DC5-5C72-4622-8027-B5A83E0C1612}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{749CF264-00C3-4BE5-B164-B2245828CF82}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{78726D1F-D52A-4979-B318-2BDFDA14F4A6}"/>
   </bookViews>
@@ -391,7 +391,7 @@
   <dimension ref="A1:D767"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>